<commit_message>
It now properly uses a calibration data file.
</commit_message>
<xml_diff>
--- a/tests/test_protocol.xlsx
+++ b/tests/test_protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab\Desktop\ph-meter-interface\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/jsb_sniprbiome_com/Documents/ph-meter-interface/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AFFFA1-1543-48A8-9180-C189686E15FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{09AFFFA1-1543-48A8-9180-C189686E15FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C45A5C-0AD9-384A-8A80-D3D8C44C4D02}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,16 +541,16 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="29" width="9.625" style="7" customWidth="1"/>
+    <col min="1" max="29" width="9.6640625" style="7" customWidth="1"/>
     <col min="30" max="32" width="11" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -600,7 +600,7 @@
       <c r="AE1"/>
       <c r="AF1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -611,7 +611,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="11">
-        <v>1440</v>
+        <v>120</v>
       </c>
       <c r="E2" s="12">
         <v>5.6</v>
@@ -623,7 +623,7 @@
         <v>300</v>
       </c>
       <c r="H2" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -650,7 +650,7 @@
       <c r="AE2"/>
       <c r="AF2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -661,7 +661,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="11">
-        <v>1440</v>
+        <v>120</v>
       </c>
       <c r="E3" s="12">
         <v>5.6</v>
@@ -673,7 +673,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -700,7 +700,7 @@
       <c r="AE3"/>
       <c r="AF3"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -711,7 +711,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="11">
-        <v>1440</v>
+        <v>120</v>
       </c>
       <c r="E4" s="12">
         <v>5.6</v>
@@ -723,7 +723,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -750,7 +750,7 @@
       <c r="AE4"/>
       <c r="AF4"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -761,7 +761,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="11">
-        <v>1440</v>
+        <v>120</v>
       </c>
       <c r="E5" s="12">
         <v>5.6</v>
@@ -773,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -800,7 +800,7 @@
       <c r="AE5"/>
       <c r="AF5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -811,7 +811,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="11">
-        <v>1440</v>
+        <v>120</v>
       </c>
       <c r="E6" s="12">
         <v>5.6</v>
@@ -823,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -850,7 +850,7 @@
       <c r="AE6"/>
       <c r="AF6"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -876,7 +876,7 @@
       <c r="AE7"/>
       <c r="AF7"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
@@ -910,7 +910,7 @@
       <c r="AE8"/>
       <c r="AF8"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="R9"/>
       <c r="S9"/>
       <c r="T9"/>
@@ -927,7 +927,7 @@
       <c r="AE9"/>
       <c r="AF9"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="R10"/>
       <c r="S10"/>
       <c r="T10"/>
@@ -944,7 +944,7 @@
       <c r="AE10"/>
       <c r="AF10"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="R11"/>
       <c r="S11"/>
       <c r="T11"/>
@@ -961,7 +961,7 @@
       <c r="AE11"/>
       <c r="AF11"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="R12"/>
       <c r="S12"/>
       <c r="T12"/>

</xml_diff>

<commit_message>
Began adding support for multitasks
</commit_message>
<xml_diff>
--- a/tests/test_protocol.xlsx
+++ b/tests/test_protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/jsb_sniprbiome_com/Documents/ph-meter-interface/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{09AFFFA1-1543-48A8-9180-C189686E15FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C45A5C-0AD9-384A-8A80-D3D8C44C4D02}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{09AFFFA1-1543-48A8-9180-C189686E15FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76AD6BA7-212C-6144-B28E-37926BAB46B2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -541,7 +541,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,11 +625,21 @@
       <c r="H2" s="13">
         <v>2</v>
       </c>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
+      <c r="I2" s="11">
+        <v>120</v>
+      </c>
+      <c r="J2" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="K2" s="12">
+        <v>8</v>
+      </c>
+      <c r="L2" s="13">
+        <v>300</v>
+      </c>
+      <c r="M2" s="13">
+        <v>2</v>
+      </c>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
@@ -675,11 +685,21 @@
       <c r="H3" s="13">
         <v>2</v>
       </c>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
+      <c r="I3" s="11">
+        <v>120</v>
+      </c>
+      <c r="J3" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="K3" s="12">
+        <v>8</v>
+      </c>
+      <c r="L3" s="13">
+        <v>10</v>
+      </c>
+      <c r="M3" s="13">
+        <v>2</v>
+      </c>
       <c r="N3"/>
       <c r="O3"/>
       <c r="P3"/>

</xml_diff>

<commit_message>
Added tests and support for restarting failed runs
</commit_message>
<xml_diff>
--- a/tests/test_protocol.xlsx
+++ b/tests/test_protocol.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/jsb_sniprbiome_com/Documents/ph-meter-interface/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jespersamsobirch/OneDrive - SniprBiome/ph-meter-interface/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{09AFFFA1-1543-48A8-9180-C189686E15FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C45A5C-0AD9-384A-8A80-D3D8C44C4D02}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBCD92D-89AC-1B45-8608-D7E038882439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -541,7 +541,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,7 +620,7 @@
         <v>6.8</v>
       </c>
       <c r="G2" s="13">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="H2" s="13">
         <v>2</v>
@@ -770,10 +770,10 @@
         <v>6.8</v>
       </c>
       <c r="G5" s="13">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H5" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -820,10 +820,10 @@
         <v>6.8</v>
       </c>
       <c r="G6" s="13">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H6" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>

</xml_diff>

<commit_message>
Added support for multitasks, but not restarting them.
</commit_message>
<xml_diff>
--- a/tests/test_protocol.xlsx
+++ b/tests/test_protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jespersamsobirch/OneDrive - SniprBiome/ph-meter-interface/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBCD92D-89AC-1B45-8608-D7E038882439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6F3A6A-CA66-304C-9926-A4177DB56C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -178,7 +178,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -193,6 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -541,7 +542,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,11 +626,21 @@
       <c r="H2" s="13">
         <v>2</v>
       </c>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
+      <c r="I2" s="11">
+        <v>90</v>
+      </c>
+      <c r="J2" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="K2" s="14">
+        <v>9</v>
+      </c>
+      <c r="L2" s="13">
+        <v>15</v>
+      </c>
+      <c r="M2" s="13">
+        <v>2</v>
+      </c>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
@@ -877,14 +888,14 @@
       <c r="AF7"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -911,6 +922,15 @@
       <c r="AF8"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
       <c r="R9"/>
       <c r="S9"/>
       <c r="T9"/>

</xml_diff>

<commit_message>
Added controllers that can properly handle dips in ph
</commit_message>
<xml_diff>
--- a/tests/test_protocol.xlsx
+++ b/tests/test_protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jespersamsobirch/OneDrive - SniprBiome/ph-meter-interface/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B80D572-507A-9344-9DEF-47260041D9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72CBC47-E556-AD4F-AB3D-837C7154046E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,7 +617,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="11">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="E2" s="12">
         <v>5.6</v>
@@ -635,7 +635,7 @@
         <v>2</v>
       </c>
       <c r="J2" s="11">
-        <v>90</v>
+        <v>700</v>
       </c>
       <c r="K2" s="14">
         <v>6.8</v>
@@ -681,7 +681,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="11">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="E3" s="12">
         <v>5.6</v>
@@ -733,7 +733,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="11">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="E4" s="12">
         <v>5.6</v>
@@ -785,7 +785,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="11">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="E5" s="12">
         <v>5.6</v>
@@ -837,7 +837,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="11">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="E6" s="12">
         <v>5.6</v>

</xml_diff>